<commit_message>
half done with first board, some bad pfets
</commit_message>
<xml_diff>
--- a/test_biases.xlsx
+++ b/test_biases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivias-local/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivias\pyvisa_instrument_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76052627-2B55-FC4A-8AA4-BCFF3B1EDE29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF46743-D815-4C9C-8373-7BAC28064C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16520" yWindow="500" windowWidth="26820" windowHeight="20320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>Biases to set (all L/W/nF)</t>
   </si>
@@ -178,6 +178,15 @@
   </si>
   <si>
     <t>0.01/0.37/0.74/1.11/1.48/1.85V</t>
+  </si>
+  <si>
+    <t>0 to -1.85V in steps of 0.01V</t>
+  </si>
+  <si>
+    <t>-0.01/-0.37/-0.74/-1.11/-1.48/-1.85V</t>
+  </si>
+  <si>
+    <t>-0.37/-0.74/-1.11/-1.48/-1.85V</t>
   </si>
 </sst>
 </file>
@@ -753,44 +762,44 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="45.5" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="14"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
       <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="19"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -798,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -806,7 +815,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -814,13 +823,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="19"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -828,7 +837,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
@@ -836,7 +845,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
@@ -844,19 +853,19 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="20"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="21"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>4</v>
       </c>
@@ -864,29 +873,29 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="21"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>4</v>
       </c>
@@ -894,20 +903,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -923,79 +932,79 @@
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1003,47 +1012,47 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>34</v>
       </c>
@@ -1051,7 +1060,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>36</v>
       </c>
@@ -1059,27 +1068,27 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>42</v>
       </c>
@@ -1090,15 +1099,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010053E15548763ABB4CA4D6860A46D77EAF" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a636c595c77536912078c5e3b083b3f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a0abc17b-26fa-4a6c-85fa-ec6ed5308116" xmlns:ns3="a6f2d9b7-3122-4fa2-9c6a-801252b48ae7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="73a89e9d907dc31e2668fc73ec36415d" ns2:_="" ns3:_="">
     <xsd:import namespace="a0abc17b-26fa-4a6c-85fa-ec6ed5308116"/>
@@ -1333,6 +1333,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1345,14 +1354,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E708609-9214-4D78-8D6D-AAC0CAAA289F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1485A619-2420-42BD-9738-34C83C002350}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1371,6 +1372,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E708609-9214-4D78-8D6D-AAC0CAAA289F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8461628B-4710-40EB-B0E0-E3ED87D2D03C}">
   <ds:schemaRefs>

</xml_diff>